<commit_message>
Commit do dia 22/7
erro na linha 220 list index out of range
</commit_message>
<xml_diff>
--- a/correcao_ppe/PROCESSOS ATUALIZADOS.xlsx
+++ b/correcao_ppe/PROCESSOS ATUALIZADOS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Antigo</t>
+          <t>Número antigo</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -461,18 +461,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>00603713620208219000</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>00364536620218219000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>71010199032</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>9051648-37.2019.8.21.0001</t>
+          <t>0050953-76.2018.8.21.0001</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0060371-36.2020.8.21.9000</t>
+          <t>0036453-66.2021.8.21.9000</t>
         </is>
       </c>
     </row>
@@ -482,18 +486,472 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>00146900920218219000</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>00201382620228219000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>71010529717</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>9016955-90.2020.8.21.0001</t>
+          <t>9006670-62.2017.8.21.0027</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0014690-09.2021.8.21.9000</t>
+          <t>0020138-26.2022.8.21.9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>00201417820228219000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>71010529741</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>9000282-12.2018.8.21.0027</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0020141-78.2022.8.21.9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>02076061920128210001</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>001/1.12.0149507-6</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sem dados do processo</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0207606-19.2012.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>00395337920158210001</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>001/1.15.0029267-3</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0131839-85.2016.8.21.7000</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0039533-79.2015.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>01271452620138210001</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>001/1.13.0109916-4</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sem dados do processo</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0127145-26.2013.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>03740784420118210001</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>001/1.11.0306661-8</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0323662-85.2015.8.21.7000</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0374078-44.2011.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>00576721120178210001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>001/1.17.0041202-8</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0283803-91.2017.8.21.7000</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0057672-11.2017.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>01480132520138210001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>001/1.13.0127652-0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Sem dados do processo</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0148013-25.2013.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>35368519520098216001</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>001/1.09.0353685-8</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0129134-27.2010.8.21.7000</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>3536851-95.2009.8.21.6001</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>34568416420098216001</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>001/1.09.0345684-6</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0168278-08.2010.8.21.7000</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>3456841-64.2009.8.21.6001</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>08374316920108216001</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>001/1.10.0083743-3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0586254-26.2011.8.21.7000</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0837431-69.2010.8.21.6001</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>90468919720198210001</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0004480-59.2022.8.21.9000</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>9046891-97.2019.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>90834124120198210001</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Sem dados do processo</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>9083412-41.2019.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>90096043220218210001</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0048164-68.2021.8.21.9000</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>9009604-32.2021.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>90240030320208210001</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Sem dados do processo</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>9024003-03.2020.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>90455096920198210001</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0021524-62.2020.8.21.9000</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>9045509-69.2019.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>00065216920188210001</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>001/3.18.0000352-3</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Sem dados do processo</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0006521-69.2018.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>00291616620188210001</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>001/3.18.0002150-5</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0054613-33.2018.8.21.7000</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0029161-66.2018.8.21.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>00730841120198210001</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>001/3.19.0001039-4</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Sem dados do processo</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0073084-11.2019.8.21.0001</t>
         </is>
       </c>
     </row>

</xml_diff>